<commit_message>
updated logboek to include woensdag
</commit_message>
<xml_diff>
--- a/Documentation/IPASS Logboek.xlsx
+++ b/Documentation/IPASS Logboek.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git_repos\IPASS_2019\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6495D3-CC57-438F-B874-86B1D2719B33}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D57EBD32-C46C-4498-BFE9-05AF051D12EE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{4E9BC45E-42C1-403B-A5CE-71024FC6D95E}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
   <si>
     <t>IPASS Xiao yi Hu</t>
   </si>
@@ -116,6 +115,57 @@
   </si>
   <si>
     <t>pin_in_out done</t>
+  </si>
+  <si>
+    <t>acknowedge bytes</t>
+  </si>
+  <si>
+    <t>major restructuring library</t>
+  </si>
+  <si>
+    <t>dummy pins</t>
+  </si>
+  <si>
+    <t>all_from_pin_out_t</t>
+  </si>
+  <si>
+    <t>acknowledge bytes weggehaald</t>
+  </si>
+  <si>
+    <t>due_remote_primitives</t>
+  </si>
+  <si>
+    <t>formatting opmooing</t>
+  </si>
+  <si>
+    <t>hc595 bitbanged spi protocol</t>
+  </si>
+  <si>
+    <t>removed hc595</t>
+  </si>
+  <si>
+    <t>port_out_from_pins_t</t>
+  </si>
+  <si>
+    <t>port_in_out_from_pins_t</t>
+  </si>
+  <si>
+    <t>port_in_from_pins_t</t>
+  </si>
+  <si>
+    <t>all_from_port_out_t</t>
+  </si>
+  <si>
+    <t>port_out primitives</t>
+  </si>
+  <si>
+    <t>all_from_pin_out_t tested</t>
+  </si>
+  <si>
+    <t>port_out_from_pins_t tested</t>
+  </si>
+  <si>
+    <t>port_in_out_from_pins_t tested</t>
   </si>
 </sst>
 </file>
@@ -512,16 +562,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF2AF77B-8E0B-44CD-A395-72E34AAED72F}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="43.5703125" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" customWidth="1"/>
     <col min="4" max="4" width="39" customWidth="1"/>
     <col min="5" max="5" width="32.85546875" customWidth="1"/>
   </cols>
@@ -666,9 +716,76 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>